<commit_message>
Prep for a run [17/06]
</commit_message>
<xml_diff>
--- a/queries/AC Cruise Speed.xlsx
+++ b/queries/AC Cruise Speed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Git 2\queries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D3B46F-3D0F-4F7F-8122-B34A1AD2FE30}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5259F5-7D18-4617-80D2-2E0C5E5FE27D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1170" windowWidth="22140" windowHeight="13305" xr2:uid="{AFB1A7AB-C8E9-469F-9139-8B73972E180E}"/>
+    <workbookView xWindow="120" yWindow="0" windowWidth="22185" windowHeight="13515" tabRatio="292" xr2:uid="{AFB1A7AB-C8E9-469F-9139-8B73972E180E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>A320</t>
   </si>
@@ -38,9 +38,6 @@
     <t>AC Type</t>
   </si>
   <si>
-    <t>Speed</t>
-  </si>
-  <si>
     <t>A321</t>
   </si>
   <si>
@@ -48,6 +45,165 @@
   </si>
   <si>
     <t>B738</t>
+  </si>
+  <si>
+    <t>FL230</t>
+  </si>
+  <si>
+    <t>FL300</t>
+  </si>
+  <si>
+    <t>FL320</t>
+  </si>
+  <si>
+    <t>FL330</t>
+  </si>
+  <si>
+    <t>FL340</t>
+  </si>
+  <si>
+    <t>FL350</t>
+  </si>
+  <si>
+    <t>FL360</t>
+  </si>
+  <si>
+    <t>FL310</t>
+  </si>
+  <si>
+    <t>A319</t>
+  </si>
+  <si>
+    <t>FL240</t>
+  </si>
+  <si>
+    <t>B734</t>
+  </si>
+  <si>
+    <t>RJ1H</t>
+  </si>
+  <si>
+    <t>B737</t>
+  </si>
+  <si>
+    <t>FL370</t>
+  </si>
+  <si>
+    <t>FL380</t>
+  </si>
+  <si>
+    <t>B736</t>
+  </si>
+  <si>
+    <t>B77W</t>
+  </si>
+  <si>
+    <t>FL220</t>
+  </si>
+  <si>
+    <t>FL210</t>
+  </si>
+  <si>
+    <t>DLH08W</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> switches FL mid cruise</t>
+  </si>
+  <si>
+    <t>DLH156</t>
+  </si>
+  <si>
+    <t>CRJ9</t>
+  </si>
+  <si>
+    <t>EIN111</t>
+  </si>
+  <si>
+    <t>B752</t>
+  </si>
+  <si>
+    <t>B733</t>
+  </si>
+  <si>
+    <t>FL170</t>
+  </si>
+  <si>
+    <t>FL180</t>
+  </si>
+  <si>
+    <t>GWI2807</t>
+  </si>
+  <si>
+    <t>FL390</t>
+  </si>
+  <si>
+    <t>skip</t>
+  </si>
+  <si>
+    <t>KLM59Z</t>
+  </si>
+  <si>
+    <t>MIBID</t>
+  </si>
+  <si>
+    <t>A332</t>
+  </si>
+  <si>
+    <t>FL400</t>
+  </si>
+  <si>
+    <t>FL410</t>
+  </si>
+  <si>
+    <t>F2TH</t>
+  </si>
+  <si>
+    <t>FL190</t>
+  </si>
+  <si>
+    <t>PGT424</t>
+  </si>
+  <si>
+    <t>QTR022</t>
+  </si>
+  <si>
+    <t>A310</t>
+  </si>
+  <si>
+    <t>FL270</t>
+  </si>
+  <si>
+    <t>RYR5008</t>
+  </si>
+  <si>
+    <t>SAS1042</t>
+  </si>
+  <si>
+    <t>SAS618</t>
+  </si>
+  <si>
+    <t>E145</t>
+  </si>
+  <si>
+    <t>FL250</t>
+  </si>
+  <si>
+    <t>B77L</t>
+  </si>
+  <si>
+    <t>TAY011</t>
+  </si>
+  <si>
+    <t>TFL219</t>
+  </si>
+  <si>
+    <t>AUA381</t>
+  </si>
+  <si>
+    <t>AUA522D</t>
+  </si>
+  <si>
+    <t>DH8D - BAD AIRCRAFT</t>
   </si>
 </sst>
 </file>
@@ -83,8 +239,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,52 +626,442 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01852D7D-15B8-4967-9EC0-885B9AE7E58A}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:X20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="E2">
+        <v>0.505</v>
+      </c>
+      <c r="F2">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="N2">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="O2">
+        <v>0.67</v>
+      </c>
+      <c r="P2">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="R2">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="S2">
+        <v>0.73</v>
+      </c>
+      <c r="T2">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="W2" t="s">
+        <v>24</v>
+      </c>
+      <c r="X2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="G3">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="H3">
+        <v>0.628</v>
+      </c>
+      <c r="K3">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="L3">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="M3">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="N3">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="O3">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="P3">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="Q3">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="R3">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="S3">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="T3">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="W3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>272.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="O4">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="P4">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="W4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>254.94900000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="G5">
+        <v>0.99</v>
+      </c>
+      <c r="L5">
+        <v>0.99</v>
+      </c>
+      <c r="W5" t="s">
+        <v>33</v>
+      </c>
+      <c r="X5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6">
+        <v>0.64</v>
+      </c>
+      <c r="W6" t="s">
+        <v>43</v>
+      </c>
+      <c r="X6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="O7">
+        <v>0.78</v>
+      </c>
+      <c r="Q7">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="R7">
+        <v>0.84</v>
+      </c>
+      <c r="W7" t="s">
+        <v>44</v>
+      </c>
+      <c r="X7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="W8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="S9">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="W9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>271.85700000000003</v>
+      <c r="C10">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="D10">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="L10">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="P10">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="Q10">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="R10">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="S10">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="T10">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="U10">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="V10">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="W10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="S11">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="W11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12">
+        <v>0.78</v>
+      </c>
+      <c r="W12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P13">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="Q13">
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="L14">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="M14">
+        <v>0.73399999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="M15">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="N15">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="O15">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="Q15">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="R15">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="S15">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="T15">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="U15">
+        <v>0.82099999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="S16">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="T16">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="U16">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="V16">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17">
+        <v>0.40899999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18">
+        <v>0.68899999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="I19">
+        <v>0.58199999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="P20">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="Q20">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="R20">
+        <v>0.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prep for a run of all Trajectories [19/06]
</commit_message>
<xml_diff>
--- a/queries/AC Cruise Speed.xlsx
+++ b/queries/AC Cruise Speed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Git 2\queries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5259F5-7D18-4617-80D2-2E0C5E5FE27D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3F66A4-2EBD-4452-8DB1-A4BA57104A11}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="0" windowWidth="22185" windowHeight="13515" tabRatio="292" xr2:uid="{AFB1A7AB-C8E9-469F-9139-8B73972E180E}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15660" tabRatio="292" xr2:uid="{AFB1A7AB-C8E9-469F-9139-8B73972E180E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>A320</t>
   </si>
@@ -107,9 +107,6 @@
     <t>DLH08W</t>
   </si>
   <si>
-    <t xml:space="preserve"> switches FL mid cruise</t>
-  </si>
-  <si>
     <t>DLH156</t>
   </si>
   <si>
@@ -204,6 +201,24 @@
   </si>
   <si>
     <t>DH8D - BAD AIRCRAFT</t>
+  </si>
+  <si>
+    <t>switch_10</t>
+  </si>
+  <si>
+    <t>switch_20</t>
+  </si>
+  <si>
+    <t>switch_30</t>
+  </si>
+  <si>
+    <t>switch_60</t>
+  </si>
+  <si>
+    <t>B763</t>
+  </si>
+  <si>
+    <t>FL290</t>
   </si>
 </sst>
 </file>
@@ -626,26 +641,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01852D7D-15B8-4967-9EC0-885B9AE7E58A}">
-  <dimension ref="A1:X20"/>
+  <dimension ref="A1:AB20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="23" max="26" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
         <v>23</v>
@@ -660,55 +679,67 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB1" t="s">
         <v>34</v>
       </c>
-      <c r="U1" t="s">
-        <v>39</v>
-      </c>
-      <c r="V1" t="s">
-        <v>40</v>
-      </c>
-      <c r="W1" t="s">
-        <v>25</v>
-      </c>
-      <c r="X1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -721,35 +752,50 @@
       <c r="F2">
         <v>0.51200000000000001</v>
       </c>
+      <c r="G2">
+        <v>0.52500000000000002</v>
+      </c>
       <c r="H2" s="1">
         <v>0.53500000000000003</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>0.65200000000000002</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0.67</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>0.68400000000000005</v>
       </c>
       <c r="R2">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="S2">
         <v>0.71899999999999997</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>0.73</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>0.74299999999999999</v>
       </c>
-      <c r="W2" t="s">
-        <v>24</v>
-      </c>
-      <c r="X2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X2">
+        <v>10</v>
+      </c>
+      <c r="Y2">
+        <v>20</v>
+      </c>
+      <c r="Z2">
+        <v>30</v>
+      </c>
+      <c r="AA2">
+        <v>60</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -762,134 +808,173 @@
       <c r="H3">
         <v>0.628</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>0.71599999999999997</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>0.73699999999999999</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>0.75700000000000001</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>0.77100000000000002</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0.78600000000000003</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>0.80200000000000005</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>0.81899999999999995</v>
-      </c>
-      <c r="R3">
-        <v>0.82099999999999995</v>
       </c>
       <c r="S3">
         <v>0.82099999999999995</v>
       </c>
       <c r="T3">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="U3">
         <v>0.88800000000000001</v>
       </c>
-      <c r="W3" t="s">
-        <v>26</v>
-      </c>
       <c r="X3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>0.77500000000000002</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>0.79100000000000004</v>
       </c>
-      <c r="W4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="G5">
         <v>0.99</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0.99</v>
       </c>
-      <c r="W5" t="s">
-        <v>33</v>
-      </c>
-      <c r="X5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>0.64</v>
       </c>
-      <c r="W6" t="s">
-        <v>43</v>
-      </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="P7">
+        <v>0.78</v>
+      </c>
+      <c r="R7">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="S7">
+        <v>0.84</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N7">
-        <v>0.75900000000000001</v>
-      </c>
-      <c r="O7">
-        <v>0.78</v>
-      </c>
-      <c r="Q7">
-        <v>0.81299999999999994</v>
-      </c>
-      <c r="R7">
-        <v>0.84</v>
-      </c>
-      <c r="W7" t="s">
-        <v>44</v>
-      </c>
-      <c r="X7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>0.79800000000000004</v>
       </c>
-      <c r="W8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>0.82099999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
+      <c r="L9">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="N9">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="O9">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="P9">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="R9">
+        <v>0.81899999999999995</v>
+      </c>
       <c r="S9">
         <v>0.82099999999999995</v>
       </c>
-      <c r="W9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="T9">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="U9">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="V9">
+        <v>0.82099999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -899,17 +984,14 @@
       <c r="D10">
         <v>0.56599999999999995</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>0.73699999999999999</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>0.80100000000000005</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>0.81899999999999995</v>
-      </c>
-      <c r="R10">
-        <v>0.82099999999999995</v>
       </c>
       <c r="S10">
         <v>0.82099999999999995</v>
@@ -918,153 +1000,130 @@
         <v>0.82099999999999995</v>
       </c>
       <c r="U10">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="V10">
         <v>0.86499999999999999</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>0.86599999999999999</v>
       </c>
-      <c r="W10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>0.82099999999999995</v>
       </c>
-      <c r="W11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>0.78</v>
       </c>
-      <c r="W12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13">
+        <v>0.746</v>
+      </c>
+      <c r="Q13">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="R13">
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>29</v>
-      </c>
-      <c r="P13">
-        <v>0.75800000000000001</v>
-      </c>
-      <c r="Q13">
-        <v>0.78200000000000003</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>30</v>
       </c>
       <c r="C14">
         <v>0.54700000000000004</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>0.71199999999999997</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>0.73399999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="K15">
-        <v>0.72399999999999998</v>
-      </c>
-      <c r="M15">
-        <v>0.76100000000000001</v>
-      </c>
-      <c r="N15">
-        <v>0.77700000000000002</v>
-      </c>
-      <c r="O15">
-        <v>0.79600000000000004</v>
-      </c>
-      <c r="Q15">
-        <v>0.81899999999999995</v>
-      </c>
-      <c r="R15">
-        <v>0.82099999999999995</v>
-      </c>
-      <c r="S15">
-        <v>0.82099999999999995</v>
+        <v>37</v>
       </c>
       <c r="T15">
-        <v>0.82099999999999995</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="U15">
-        <v>0.82099999999999995</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="V15">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="W15">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
-      </c>
-      <c r="S16">
-        <v>0.85899999999999999</v>
-      </c>
-      <c r="T16">
-        <v>0.85899999999999999</v>
-      </c>
-      <c r="U16">
-        <v>0.85899999999999999</v>
-      </c>
-      <c r="V16">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="D16">
+        <v>0.40899999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17">
-        <v>0.40899999999999997</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="J17">
+        <v>0.68899999999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="J18">
-        <v>0.68899999999999995</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="H18">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="I18">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="K18">
+        <v>0.64100000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
-      </c>
-      <c r="H19">
-        <v>0.57099999999999995</v>
-      </c>
-      <c r="I19">
-        <v>0.58199999999999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="Q19">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="R19">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="S19">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
-      </c>
-      <c r="P20">
-        <v>0.80100000000000005</v>
-      </c>
-      <c r="Q20">
-        <v>0.81299999999999994</v>
-      </c>
-      <c r="R20">
-        <v>0.84</v>
+        <v>61</v>
+      </c>
+      <c r="T20">
+        <v>0.86099999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Latest Version 1 [09/07]
</commit_message>
<xml_diff>
--- a/queries/AC Cruise Speed.xlsx
+++ b/queries/AC Cruise Speed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Git 2\queries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8B4090-BF6C-44AA-A6FC-4454516FA7AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB9F764-65D3-4151-AA83-F61BC2460899}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="1800" windowWidth="28695" windowHeight="13515" tabRatio="292" xr2:uid="{AFB1A7AB-C8E9-469F-9139-8B73972E180E}"/>
+    <workbookView xWindow="1230" yWindow="2985" windowWidth="27570" windowHeight="12555" tabRatio="292" xr2:uid="{AFB1A7AB-C8E9-469F-9139-8B73972E180E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -643,12 +643,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01852D7D-15B8-4967-9EC0-885B9AE7E58A}">
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AB4" sqref="AB4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="14" width="9.140625" customWidth="1"/>
     <col min="23" max="26" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -830,13 +831,13 @@
         <v>0.81899999999999995</v>
       </c>
       <c r="S3">
-        <v>0.82099999999999995</v>
+        <v>0.82</v>
       </c>
       <c r="T3">
-        <v>0.82099999999999995</v>
+        <v>0.82</v>
       </c>
       <c r="U3">
-        <v>0.88800000000000001</v>
+        <v>0.82</v>
       </c>
       <c r="X3" t="s">
         <v>24</v>
@@ -885,10 +886,10 @@
         <v>3</v>
       </c>
       <c r="G5">
-        <v>0.99</v>
+        <v>0.65400000000000003</v>
       </c>
       <c r="M5">
-        <v>0.99</v>
+        <v>0.66</v>
       </c>
       <c r="Y5" t="s">
         <v>47</v>
@@ -942,7 +943,7 @@
         <v>0.79800000000000004</v>
       </c>
       <c r="Q8">
-        <v>0.82099999999999995</v>
+        <v>0.81899999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -965,16 +966,16 @@
         <v>0.81899999999999995</v>
       </c>
       <c r="S9">
-        <v>0.82099999999999995</v>
+        <v>0.81899999999999995</v>
       </c>
       <c r="T9">
-        <v>0.82099999999999995</v>
+        <v>0.81899999999999995</v>
       </c>
       <c r="U9">
-        <v>0.82099999999999995</v>
+        <v>0.81899999999999995</v>
       </c>
       <c r="V9">
-        <v>0.82099999999999995</v>
+        <v>0.81899999999999995</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -997,19 +998,19 @@
         <v>0.81899999999999995</v>
       </c>
       <c r="S10">
-        <v>0.82099999999999995</v>
+        <v>0.82</v>
       </c>
       <c r="T10">
-        <v>0.82099999999999995</v>
+        <v>0.81899999999999995</v>
       </c>
       <c r="U10">
-        <v>0.82099999999999995</v>
+        <v>0.81899999999999995</v>
       </c>
       <c r="V10">
-        <v>0.86499999999999999</v>
+        <v>0.82</v>
       </c>
       <c r="W10">
-        <v>0.86599999999999999</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -1017,7 +1018,7 @@
         <v>20</v>
       </c>
       <c r="T11">
-        <v>0.82099999999999995</v>
+        <v>0.81899999999999995</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -1070,7 +1071,7 @@
         <v>0.85899999999999999</v>
       </c>
       <c r="W15">
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -1122,7 +1123,7 @@
         <v>61</v>
       </c>
       <c r="T20">
-        <v>0.86099999999999999</v>
+        <v>0.85899999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>